<commit_message>
Done Fixing Uploading and Auto-cost of Employe
</commit_message>
<xml_diff>
--- a/manpower_adjustment/templates/Manpower Adjustment Template.xlsx
+++ b/manpower_adjustment/templates/Manpower Adjustment Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAS\Desktop\SAS Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\shuttle_allocation\manpower_adjustment\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25308EA2-E093-47CD-B02B-9D020BEB7BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BBB7EB-3D0D-4BB8-94AC-DFFF1DDA0567}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Employee" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="410">
   <si>
     <t>ID Number</t>
   </si>
@@ -1246,36 +1246,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>MAZDA_J12A</t>
-  </si>
-  <si>
-    <t>HONDA</t>
-  </si>
-  <si>
-    <t>MAZDA MERGE</t>
-  </si>
-  <si>
-    <t>SUZUKI</t>
-  </si>
-  <si>
-    <t>TOYOTA</t>
-  </si>
-  <si>
-    <t>DAIHATSU</t>
-  </si>
-  <si>
-    <t>SUBARU</t>
-  </si>
-  <si>
-    <t>NISSAN</t>
-  </si>
-  <si>
-    <t>DAIHATSU_D01L</t>
-  </si>
-  <si>
-    <t>HONDA_TKRA</t>
   </si>
   <si>
     <t>Job Type</t>
@@ -1336,11 +1306,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1714,10 +1686,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1734,13 +1706,12 @@
     <col min="12" max="12" width="31.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.28515625" style="4" customWidth="1"/>
     <col min="14" max="15" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="4"/>
-    <col min="18" max="18" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="4"/>
+    <col min="16" max="16" width="14.42578125" style="4"/>
+    <col min="17" max="17" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1783,25 +1754,22 @@
         <v>44</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1828,9 +1796,8 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-    </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1847,9 +1814,8 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1866,9 +1832,8 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1885,9 +1850,8 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1904,9 +1868,8 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1923,9 +1886,8 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1942,9 +1904,8 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1961,9 +1922,8 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1980,9 +1940,8 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1999,9 +1958,8 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2018,9 +1976,8 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2037,9 +1994,8 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2057,9 +2013,8 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2078,9 +2033,8 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2098,11 +2052,10 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S16" s="3"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2120,11 +2073,10 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S17" s="3"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2142,11 +2094,10 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="3"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2165,9 +2116,8 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2186,9 +2136,8 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-    </row>
-    <row r="21" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2207,9 +2156,8 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-    </row>
-    <row r="22" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2228,9 +2176,8 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-    </row>
-    <row r="23" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2249,9 +2196,8 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-    </row>
-    <row r="24" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2270,9 +2216,8 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-    </row>
-    <row r="25" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2291,9 +2236,8 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-    </row>
-    <row r="26" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2312,9 +2256,8 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-    </row>
-    <row r="27" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2333,9 +2276,8 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2354,9 +2296,8 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2375,9 +2316,8 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-    </row>
-    <row r="30" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2396,9 +2336,8 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-    </row>
-    <row r="31" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2417,9 +2356,8 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-    </row>
-    <row r="32" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2438,9 +2376,8 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-    </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2459,9 +2396,8 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2480,9 +2416,8 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-    </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2501,9 +2436,8 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2522,9 +2456,8 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2543,9 +2476,8 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-    </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2564,9 +2496,8 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-    </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2585,9 +2516,8 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-    </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2606,9 +2536,8 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-    </row>
-    <row r="41" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2627,9 +2556,8 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-    </row>
-    <row r="42" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2648,9 +2576,8 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-    </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2669,9 +2596,8 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-    </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2690,9 +2616,8 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-    </row>
-    <row r="45" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2711,9 +2636,8 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-    </row>
-    <row r="46" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2732,17 +2656,21 @@
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="K1:K46" xr:uid="{5BD93150-2408-4919-94E3-1FF0CBEA5F76}"/>
-  <mergeCells count="19">
-    <mergeCell ref="U1:U2"/>
+  <mergeCells count="18">
+    <mergeCell ref="T1:T2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:F1"/>
@@ -2751,16 +2679,10 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="P1:P2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{441111BF-EABA-4FD0-86D8-997766137D19}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576" xr:uid="{441111BF-EABA-4FD0-86D8-997766137D19}">
       <formula1>"A,B"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{E69203C7-1D77-4523-8ABC-D9E309239DF4}">
@@ -2782,7 +2704,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09B9F990-1765-4451-B88F-CBB59DDA2C07}">
           <x14:formula1>
             <xm:f>Reference!$A$2:$A$13</xm:f>
@@ -2805,25 +2727,19 @@
           <x14:formula1>
             <xm:f>Reference!$G$2:$G$15</xm:f>
           </x14:formula1>
-          <xm:sqref>R1:R1048576</xm:sqref>
+          <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE78EA92-9F18-4706-AF90-562C32C1B896}">
           <x14:formula1>
             <xm:f>Reference!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>S1:S1048576</xm:sqref>
+          <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D1F06C8-73A0-48D9-BDF4-BAC1FB9ACBF0}">
           <x14:formula1>
             <xm:f>Reference!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T1:T1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2BF5850-9B66-4399-A1B6-DAFAFFC3938D}">
-          <x14:formula1>
-            <xm:f>Reference!$K$2:$K$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>P1:P1048576</xm:sqref>
+          <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90914595-72DB-4F65-BA47-DE1FD9C729A3}">
           <x14:formula1>
@@ -2845,9 +2761,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D25D0AB1-C430-473D-96A4-A8A65EFC3D38}">
           <x14:formula1>
-            <xm:f>Reference!$L$2:$L$3</xm:f>
+            <xm:f>Reference!$K$2:$K$3</xm:f>
           </x14:formula1>
-          <xm:sqref>U1:U1048576</xm:sqref>
+          <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2860,10 +2776,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L357"/>
+  <dimension ref="A1:K357"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2794,7 @@
     <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2910,13 +2826,10 @@
         <v>403</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -2947,14 +2860,11 @@
       <c r="J2" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="K2" t="s">
-        <v>406</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2985,14 +2895,11 @@
       <c r="J3" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="K3" t="s">
-        <v>407</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
@@ -3016,11 +2923,8 @@
         <v>26</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="K4" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -3042,16 +2946,13 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>275</v>
@@ -3068,11 +2969,8 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="K6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>30</v>
       </c>
@@ -3094,11 +2992,8 @@
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="K7" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>31</v>
       </c>
@@ -3118,11 +3013,8 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="K8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -3142,11 +3034,8 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="K9" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>349</v>
       </c>
@@ -3166,11 +3055,8 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="K10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
@@ -3190,11 +3076,8 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="K11" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
@@ -3215,7 +3098,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -3236,7 +3119,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
@@ -3257,7 +3140,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="11" t="s">
@@ -3276,7 +3159,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="11" t="s">
@@ -6657,7 +6540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98482112-5248-40D3-ADB8-C4A981BC2DB6}">
   <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+    <sheetView topLeftCell="A191" workbookViewId="0">
       <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>

</xml_diff>